<commit_message>
Updated hex values of beq and bne
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-45" yWindow="30" windowWidth="26100" windowHeight="12735"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
   <si>
     <t>OpCode [31 : 26]</t>
   </si>
@@ -318,25 +318,28 @@
     <t>0x3C160028</t>
   </si>
   <si>
-    <t>504-600</t>
-  </si>
-  <si>
-    <t>604-700</t>
-  </si>
-  <si>
-    <t>0-500</t>
+    <t>(1000)0000001111101000</t>
+  </si>
+  <si>
+    <t>0x12AE03E8</t>
+  </si>
+  <si>
+    <t>(1248)0000010011100000</t>
+  </si>
+  <si>
+    <t>0x16AE04E0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="000000"/>
     <numFmt numFmtId="165" formatCode="000\100"/>
     <numFmt numFmtId="166" formatCode="00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,19 +348,13 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -621,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -670,9 +667,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,16 +703,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -749,6 +734,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -840,7 +828,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -875,7 +862,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1051,14 +1037,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -1078,7 +1064,7 @@
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="4">
         <v>100011</v>
       </c>
@@ -1115,7 +1101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="4">
         <v>101011</v>
       </c>
@@ -1132,7 +1118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -1149,7 +1135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -1166,10 +1152,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="2">
         <v>101</v>
       </c>
@@ -1186,7 +1172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="2">
         <v>1111</v>
       </c>
@@ -1203,8 +1189,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="11" spans="1:16">
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -1224,7 +1210,7 @@
       <c r="O11" s="8"/>
       <c r="P11" s="9"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1257,11 +1243,11 @@
       <c r="O12" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="44" t="s">
+      <c r="P12" s="40" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1285,14 +1271,14 @@
       <c r="L13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="44"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="40"/>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1308,14 +1294,14 @@
         <v>61</v>
       </c>
       <c r="J14" s="15"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="44"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K14" s="43"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="40"/>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1325,34 +1311,34 @@
       <c r="C15" s="1">
         <v>100</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="J15" s="22" t="s">
+      <c r="I15" s="20">
+        <v>512</v>
+      </c>
+      <c r="J15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="L15" s="22" t="s">
+      <c r="L15" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="M15" s="49" t="s">
+      <c r="M15" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="N15" s="49"/>
-      <c r="O15" s="50"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="46"/>
       <c r="P15" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1362,34 +1348,34 @@
       <c r="C16" s="1">
         <v>110</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="G16" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="J16" s="22" t="s">
+      <c r="I16" s="20">
+        <v>648</v>
+      </c>
+      <c r="J16" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="49" t="s">
+      <c r="M16" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="N16" s="49"/>
-      <c r="O16" s="50"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="46"/>
       <c r="P16" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1399,38 +1385,38 @@
       <c r="C17" s="1">
         <v>120</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="I17" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="J17" s="28" t="s">
+      <c r="I17" s="20">
+        <v>16</v>
+      </c>
+      <c r="J17" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="N17" s="23" t="s">
+      <c r="N17" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="O17" s="24" t="s">
+      <c r="O17" s="23" t="s">
         <v>79</v>
       </c>
       <c r="P17" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1440,30 +1426,34 @@
       <c r="C18" s="1">
         <v>130</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="I18" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="J18" s="29" t="s">
+      <c r="I18" s="20">
+        <v>24</v>
+      </c>
+      <c r="J18" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="K18" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="18"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M18" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="N18" s="45"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1473,18 +1463,18 @@
       <c r="C19" s="1">
         <v>140</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
       <c r="P19" s="16"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1494,30 +1484,34 @@
       <c r="C20" s="1">
         <v>150</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="20">
+        <v>32</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="L20" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="M20" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="J20" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="L20" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="19"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="45"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -1527,34 +1521,34 @@
       <c r="C21" s="1">
         <v>160</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="J21" s="30" t="s">
+      <c r="I21" s="47">
+        <v>40</v>
+      </c>
+      <c r="J21" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="K21" s="27" t="s">
+      <c r="K21" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="M21" s="41" t="s">
+      <c r="M21" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="N21" s="41"/>
-      <c r="O21" s="42"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38"/>
       <c r="P21" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1565,7 +1559,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -1576,7 +1570,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1587,7 +1581,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1598,7 +1592,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
@@ -1609,7 +1603,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -1619,11 +1613,11 @@
       <c r="C27" s="1">
         <v>220</v>
       </c>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
@@ -1634,7 +1628,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
         <v>57</v>
       </c>
@@ -1645,7 +1639,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -1673,24 +1667,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated bunch of stuff
Added Overall TestBench, fixed other test bench issues, renamed
ICache_System file and test_bench, Updated data flow diagram
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:H21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>